<commit_message>
add experiment; adjust original script
</commit_message>
<xml_diff>
--- a/experiment/rawData.xlsx
+++ b/experiment/rawData.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizi/Desktop/pl/getprime/experiment/dbsize/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lizi/Desktop/pl/getprime/experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0186568-1C51-9B47-A2AC-CBF3CA5ECF9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A8E30C4-69A3-6D47-BAEF-32075CF09D19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15520" xr2:uid="{16D82FB4-5617-EC48-B6EB-8E37FADD908D}"/>
+    <workbookView xWindow="3800" yWindow="500" windowWidth="21800" windowHeight="15500" xr2:uid="{16D82FB4-5617-EC48-B6EB-8E37FADD908D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
   <si>
     <t>fwd-100</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -118,6 +118,14 @@
   </si>
   <si>
     <t>bwd-20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fwd-5000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bwd-5000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -484,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCB3D721-CB30-4E4E-9F0D-9AF13F5D8677}">
   <dimension ref="A1:AW15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AP12" sqref="AP12"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -509,9 +517,15 @@
         <v>3</v>
       </c>
       <c r="Z2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL2" t="s">
         <v>4</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AR2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -624,6 +638,42 @@
       <c r="AK3" t="s">
         <v>10</v>
       </c>
+      <c r="AL3">
+        <v>1</v>
+      </c>
+      <c r="AM3">
+        <v>2</v>
+      </c>
+      <c r="AN3">
+        <v>3</v>
+      </c>
+      <c r="AO3">
+        <v>4</v>
+      </c>
+      <c r="AP3">
+        <v>5</v>
+      </c>
+      <c r="AQ3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AR3">
+        <v>1</v>
+      </c>
+      <c r="AS3">
+        <v>2</v>
+      </c>
+      <c r="AT3">
+        <v>3</v>
+      </c>
+      <c r="AU3">
+        <v>4</v>
+      </c>
+      <c r="AV3">
+        <v>5</v>
+      </c>
+      <c r="AW3" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:49">
       <c r="A4" t="s">
@@ -706,41 +756,79 @@
         <v>1.5376000000000001E-3</v>
       </c>
       <c r="Z4">
-        <v>1.5506000000000001E-2</v>
+        <v>7.326E-3</v>
       </c>
       <c r="AA4">
-        <v>1.8748000000000001E-2</v>
+        <v>6.7530000000000003E-3</v>
       </c>
       <c r="AB4">
-        <v>1.7437000000000001E-2</v>
+        <v>6.8630000000000002E-3</v>
       </c>
       <c r="AC4">
-        <v>1.9994999999999999E-2</v>
+        <v>7.1529999999999996E-3</v>
       </c>
       <c r="AD4">
-        <v>1.9238999999999999E-2</v>
+        <v>1.0432E-2</v>
       </c>
       <c r="AE4">
         <f>AVERAGE(Z4:AD4)</f>
-        <v>1.8185E-2</v>
+        <v>7.7054000000000011E-3</v>
       </c>
       <c r="AF4">
-        <v>1.6677999999999998E-2</v>
+        <v>6.8180000000000003E-3</v>
       </c>
       <c r="AG4">
-        <v>1.9002000000000002E-2</v>
+        <v>6.4120000000000002E-3</v>
       </c>
       <c r="AH4">
-        <v>1.6296000000000001E-2</v>
+        <v>6.6470000000000001E-3</v>
       </c>
       <c r="AI4">
-        <v>1.2933E-2</v>
+        <v>6.3509999999999999E-3</v>
       </c>
       <c r="AJ4">
-        <v>1.7891000000000001E-2</v>
+        <v>9.1529999999999997E-3</v>
       </c>
       <c r="AK4">
         <f>AVERAGE(AF4:AJ4)</f>
+        <v>7.0761999999999995E-3</v>
+      </c>
+      <c r="AL4">
+        <v>1.5506000000000001E-2</v>
+      </c>
+      <c r="AM4">
+        <v>1.8748000000000001E-2</v>
+      </c>
+      <c r="AN4">
+        <v>1.7437000000000001E-2</v>
+      </c>
+      <c r="AO4">
+        <v>1.9994999999999999E-2</v>
+      </c>
+      <c r="AP4">
+        <v>1.9238999999999999E-2</v>
+      </c>
+      <c r="AQ4">
+        <f>AVERAGE(AL4:AP4)</f>
+        <v>1.8185E-2</v>
+      </c>
+      <c r="AR4">
+        <v>1.6677999999999998E-2</v>
+      </c>
+      <c r="AS4">
+        <v>1.9002000000000002E-2</v>
+      </c>
+      <c r="AT4">
+        <v>1.6296000000000001E-2</v>
+      </c>
+      <c r="AU4">
+        <v>1.2933E-2</v>
+      </c>
+      <c r="AV4">
+        <v>1.7891000000000001E-2</v>
+      </c>
+      <c r="AW4">
+        <f>AVERAGE(AR4:AV4)</f>
         <v>1.6560000000000002E-2</v>
       </c>
     </row>
@@ -825,41 +913,79 @@
         <v>2.2334E-3</v>
       </c>
       <c r="Z5">
+        <v>4.6560000000000004E-3</v>
+      </c>
+      <c r="AA5">
+        <v>4.424E-3</v>
+      </c>
+      <c r="AB5">
+        <v>4.1850000000000004E-3</v>
+      </c>
+      <c r="AC5">
+        <v>4.1120000000000002E-3</v>
+      </c>
+      <c r="AD5">
+        <v>4.4929999999999996E-3</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" ref="AE5:AE7" si="3">AVERAGE(Z5:AD5)</f>
+        <v>4.3740000000000012E-3</v>
+      </c>
+      <c r="AF5">
+        <v>1.4656000000000001E-2</v>
+      </c>
+      <c r="AG5">
+        <v>1.0240000000000001E-2</v>
+      </c>
+      <c r="AH5">
+        <v>1.4090999999999999E-2</v>
+      </c>
+      <c r="AI5">
+        <v>1.031E-2</v>
+      </c>
+      <c r="AJ5">
+        <v>1.3845E-2</v>
+      </c>
+      <c r="AK5">
+        <f t="shared" ref="AK5:AK7" si="4">AVERAGE(AF5:AJ5)</f>
+        <v>1.2628400000000001E-2</v>
+      </c>
+      <c r="AL5">
         <v>7.757E-3</v>
       </c>
-      <c r="AA5">
+      <c r="AM5">
         <v>8.1060000000000004E-3</v>
       </c>
-      <c r="AB5">
+      <c r="AN5">
         <v>8.5249999999999996E-3</v>
       </c>
-      <c r="AC5">
+      <c r="AO5">
         <v>7.7629999999999999E-3</v>
       </c>
-      <c r="AD5">
+      <c r="AP5">
         <v>8.2749999999999994E-3</v>
       </c>
-      <c r="AE5">
-        <f t="shared" ref="AE5:AE15" si="3">AVERAGE(Z5:AD5)</f>
+      <c r="AQ5">
+        <f>AVERAGE(AL5:AP5)</f>
         <v>8.085199999999999E-3</v>
       </c>
-      <c r="AF5">
+      <c r="AR5">
         <v>2.4788999999999999E-2</v>
       </c>
-      <c r="AG5">
+      <c r="AS5">
         <v>2.3602999999999999E-2</v>
       </c>
-      <c r="AH5">
+      <c r="AT5">
         <v>2.5687000000000001E-2</v>
       </c>
-      <c r="AI5">
+      <c r="AU5">
         <v>2.3106999999999999E-2</v>
       </c>
-      <c r="AJ5">
+      <c r="AV5">
         <v>2.8437E-2</v>
       </c>
-      <c r="AK5">
-        <f t="shared" ref="AK5:AK15" si="4">AVERAGE(AF5:AJ5)</f>
+      <c r="AW5">
+        <f>AVERAGE(AR5:AV5)</f>
         <v>2.5124600000000004E-2</v>
       </c>
     </row>
@@ -944,41 +1070,79 @@
         <v>7.4176000000000008E-3</v>
       </c>
       <c r="Z6">
-        <v>6.2507999999999994E-2</v>
+        <v>2.8778999999999999E-2</v>
       </c>
       <c r="AA6">
-        <v>5.7099999999999998E-2</v>
+        <v>2.5654E-2</v>
       </c>
       <c r="AB6">
-        <v>4.9230999999999997E-2</v>
+        <v>2.9052999999999999E-2</v>
       </c>
       <c r="AC6">
-        <v>5.2032000000000002E-2</v>
+        <v>2.6107000000000002E-2</v>
       </c>
       <c r="AD6">
-        <v>5.3022E-2</v>
+        <v>2.9322000000000001E-2</v>
       </c>
       <c r="AE6">
         <f t="shared" si="3"/>
-        <v>5.4778599999999997E-2</v>
+        <v>2.7783000000000002E-2</v>
       </c>
       <c r="AF6">
-        <v>7.1325E-2</v>
+        <v>3.7707999999999998E-2</v>
       </c>
       <c r="AG6">
-        <v>7.6974000000000001E-2</v>
+        <v>3.5338000000000001E-2</v>
       </c>
       <c r="AH6">
-        <v>7.1873999999999993E-2</v>
+        <v>3.9655999999999997E-2</v>
       </c>
       <c r="AI6">
-        <v>6.93E-2</v>
+        <v>3.8644999999999999E-2</v>
       </c>
       <c r="AJ6">
-        <v>7.2987999999999997E-2</v>
+        <v>3.9336999999999997E-2</v>
       </c>
       <c r="AK6">
         <f t="shared" si="4"/>
+        <v>3.8136800000000005E-2</v>
+      </c>
+      <c r="AL6">
+        <v>6.2507999999999994E-2</v>
+      </c>
+      <c r="AM6">
+        <v>5.7099999999999998E-2</v>
+      </c>
+      <c r="AN6">
+        <v>4.9230999999999997E-2</v>
+      </c>
+      <c r="AO6">
+        <v>5.2032000000000002E-2</v>
+      </c>
+      <c r="AP6">
+        <v>5.3022E-2</v>
+      </c>
+      <c r="AQ6">
+        <f>AVERAGE(AL6:AP6)</f>
+        <v>5.4778599999999997E-2</v>
+      </c>
+      <c r="AR6">
+        <v>7.1325E-2</v>
+      </c>
+      <c r="AS6">
+        <v>7.6974000000000001E-2</v>
+      </c>
+      <c r="AT6">
+        <v>7.1873999999999993E-2</v>
+      </c>
+      <c r="AU6">
+        <v>6.93E-2</v>
+      </c>
+      <c r="AV6">
+        <v>7.2987999999999997E-2</v>
+      </c>
+      <c r="AW6">
+        <f>AVERAGE(AR6:AV6)</f>
         <v>7.2492199999999993E-2</v>
       </c>
     </row>
@@ -1063,41 +1227,79 @@
         <v>5.104E-3</v>
       </c>
       <c r="Z7">
-        <v>5.0009999999999999E-2</v>
+        <v>2.4795000000000001E-2</v>
       </c>
       <c r="AA7">
-        <v>4.5608000000000003E-2</v>
+        <v>2.3858000000000001E-2</v>
       </c>
       <c r="AB7">
-        <v>4.5345000000000003E-2</v>
+        <v>2.2079000000000001E-2</v>
       </c>
       <c r="AC7">
-        <v>5.0296E-2</v>
+        <v>2.1486999999999999E-2</v>
       </c>
       <c r="AD7">
-        <v>4.6237E-2</v>
+        <v>2.3858000000000001E-2</v>
       </c>
       <c r="AE7">
         <f t="shared" si="3"/>
-        <v>4.7499200000000005E-2</v>
+        <v>2.3215400000000001E-2</v>
       </c>
       <c r="AF7">
-        <v>4.3097000000000003E-2</v>
+        <v>2.1187000000000001E-2</v>
       </c>
       <c r="AG7">
-        <v>4.1549000000000003E-2</v>
+        <v>2.1586000000000001E-2</v>
       </c>
       <c r="AH7">
-        <v>4.555E-2</v>
+        <v>2.188E-2</v>
       </c>
       <c r="AI7">
-        <v>4.1374000000000001E-2</v>
+        <v>2.5700000000000001E-2</v>
       </c>
       <c r="AJ7">
-        <v>4.1378999999999999E-2</v>
+        <v>2.4653000000000001E-2</v>
       </c>
       <c r="AK7">
         <f t="shared" si="4"/>
+        <v>2.3001199999999999E-2</v>
+      </c>
+      <c r="AL7">
+        <v>5.0009999999999999E-2</v>
+      </c>
+      <c r="AM7">
+        <v>4.5608000000000003E-2</v>
+      </c>
+      <c r="AN7">
+        <v>4.5345000000000003E-2</v>
+      </c>
+      <c r="AO7">
+        <v>5.0296E-2</v>
+      </c>
+      <c r="AP7">
+        <v>4.6237E-2</v>
+      </c>
+      <c r="AQ7">
+        <f>AVERAGE(AL7:AP7)</f>
+        <v>4.7499200000000005E-2</v>
+      </c>
+      <c r="AR7">
+        <v>4.3097000000000003E-2</v>
+      </c>
+      <c r="AS7">
+        <v>4.1549000000000003E-2</v>
+      </c>
+      <c r="AT7">
+        <v>4.555E-2</v>
+      </c>
+      <c r="AU7">
+        <v>4.1374000000000001E-2</v>
+      </c>
+      <c r="AV7">
+        <v>4.1378999999999999E-2</v>
+      </c>
+      <c r="AW7">
+        <f>AVERAGE(AR7:AV7)</f>
         <v>4.2589799999999997E-2</v>
       </c>
     </row>
@@ -1374,7 +1576,7 @@
         <v>5.4912999999999997E-2</v>
       </c>
       <c r="AE12">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="AE5:AE15" si="5">AVERAGE(Z12:AD12)</f>
         <v>5.9025800000000003E-2</v>
       </c>
       <c r="AF12">
@@ -1393,7 +1595,7 @@
         <v>5.323E-2</v>
       </c>
       <c r="AK12">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="AK5:AK15" si="6">AVERAGE(AF12:AJ12)</f>
         <v>5.6750800000000004E-2</v>
       </c>
       <c r="AL12">
@@ -1455,7 +1657,7 @@
         <v>2.5288000000000001E-2</v>
       </c>
       <c r="G13">
-        <f t="shared" ref="G13:G15" si="5">AVERAGE(B13:F13)</f>
+        <f t="shared" ref="G13:G15" si="7">AVERAGE(B13:F13)</f>
         <v>2.5720799999999999E-2</v>
       </c>
       <c r="H13">
@@ -1531,7 +1733,7 @@
         <v>0.17952299999999999</v>
       </c>
       <c r="AE13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.18079019999999998</v>
       </c>
       <c r="AF13">
@@ -1550,7 +1752,7 @@
         <v>0.120425</v>
       </c>
       <c r="AK13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.12163500000000001</v>
       </c>
       <c r="AL13">
@@ -1569,7 +1771,7 @@
         <v>0.254498</v>
       </c>
       <c r="AQ13">
-        <f t="shared" ref="AQ13:AQ15" si="6">AVERAGE(AL13:AP13)</f>
+        <f t="shared" ref="AQ13:AQ15" si="8">AVERAGE(AL13:AP13)</f>
         <v>0.2586328</v>
       </c>
       <c r="AR13">
@@ -1588,7 +1790,7 @@
         <v>0.151976</v>
       </c>
       <c r="AW13">
-        <f t="shared" ref="AW13:AW15" si="7">AVERAGE(AR13:AV13)</f>
+        <f t="shared" ref="AW13:AW15" si="9">AVERAGE(AR13:AV13)</f>
         <v>0.15873180000000001</v>
       </c>
     </row>
@@ -1612,7 +1814,7 @@
         <v>9.5776E-2</v>
       </c>
       <c r="G14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>9.7882399999999994E-2</v>
       </c>
       <c r="H14">
@@ -1688,7 +1890,7 @@
         <v>0.23661799999999999</v>
       </c>
       <c r="AE14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.2404394</v>
       </c>
       <c r="AF14">
@@ -1707,7 +1909,7 @@
         <v>0.421732</v>
       </c>
       <c r="AK14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.42814259999999998</v>
       </c>
       <c r="AL14">
@@ -1726,7 +1928,7 @@
         <v>0.27466499999999999</v>
       </c>
       <c r="AQ14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.27479399999999998</v>
       </c>
       <c r="AR14">
@@ -1745,7 +1947,7 @@
         <v>0.595306</v>
       </c>
       <c r="AW14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.59599820000000003</v>
       </c>
     </row>
@@ -1769,7 +1971,7 @@
         <v>7.2335999999999998E-2</v>
       </c>
       <c r="G15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v>7.0268799999999992E-2</v>
       </c>
       <c r="H15">
@@ -1845,7 +2047,7 @@
         <v>0.18137</v>
       </c>
       <c r="AE15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0.18239960000000002</v>
       </c>
       <c r="AF15">
@@ -1864,7 +2066,7 @@
         <v>0.23179900000000001</v>
       </c>
       <c r="AK15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0.228269</v>
       </c>
       <c r="AL15">
@@ -1883,7 +2085,7 @@
         <v>0.237072</v>
       </c>
       <c r="AQ15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.231346</v>
       </c>
       <c r="AR15">
@@ -1902,7 +2104,7 @@
         <v>0.31387999999999999</v>
       </c>
       <c r="AW15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.30895079999999997</v>
       </c>
     </row>

</xml_diff>